<commit_message>
Add IndexUsageAndKeyOrdering plus fixes to IndexInfo and StatisticsInfo
</commit_message>
<xml_diff>
--- a/DMV/ExcelTemplates/InstanceInfo.xlsx
+++ b/DMV/ExcelTemplates/InstanceInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\GitHub\SQLServerPerformanceTuning\ExcelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\SQLServerPerformanceTuning\DMV\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE11C16-7796-47BE-82D4-8500823DB302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6C5835-E948-4687-9F83-6BC5F89564AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{10AD8C71-7510-4E2A-9097-D6D1B55202C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10AD8C71-7510-4E2A-9097-D6D1B55202C8}"/>
   </bookViews>
   <sheets>
     <sheet name="SysInfo" sheetId="5" r:id="rId1"/>
@@ -22,12 +22,13 @@
     <sheet name="IndexInfo" sheetId="8" r:id="rId7"/>
     <sheet name="IndexUsage" sheetId="9" r:id="rId8"/>
     <sheet name="IndexOps" sheetId="10" r:id="rId9"/>
-    <sheet name="StatisticsInfo" sheetId="11" r:id="rId10"/>
-    <sheet name="StatisticsHistogram" sheetId="12" r:id="rId11"/>
+    <sheet name="IndexKeyOrdering" sheetId="13" r:id="rId10"/>
+    <sheet name="StatisticsInfo" sheetId="11" r:id="rId11"/>
+    <sheet name="StatisticsHistogram" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="189">
   <si>
     <t>server_name</t>
   </si>
@@ -592,6 +593,30 @@
   </si>
   <si>
     <t>visible_target_mb</t>
+  </si>
+  <si>
+    <t>key_ordinal</t>
+  </si>
+  <si>
+    <t>column_name</t>
+  </si>
+  <si>
+    <t>avg_distribution</t>
+  </si>
+  <si>
+    <t>max_distribution</t>
+  </si>
+  <si>
+    <t>avg_distribution_order</t>
+  </si>
+  <si>
+    <t>max_distribution_order</t>
+  </si>
+  <si>
+    <t>order_issue_avg_dist</t>
+  </si>
+  <si>
+    <t>order_issue_max_dist</t>
   </si>
 </sst>
 </file>
@@ -630,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -638,11 +663,36 @@
     </xf>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="29" formatCode="mm:ss.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
     </dxf>
@@ -669,9 +719,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="29" formatCode="mm:ss.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
@@ -1003,7 +1050,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE0AA7EF-212B-45A0-B90F-79529C042135}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="schema_object_name">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE0AA7EF-212B-45A0-B90F-79529C042135}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="schema_object_name">
   <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
@@ -1323,7 +1370,7 @@
     <tableColumn id="16" xr3:uid="{E1A234A1-E64F-46B7-B885-8606FEE8A597}" name="scheduler_total_count"/>
     <tableColumn id="17" xr3:uid="{FEBFF05F-A9CF-4223-9792-0ADA879F81A6}" name="deadlock_monitor_serial_number"/>
     <tableColumn id="18" xr3:uid="{793249C1-FF6B-4CE4-996B-76BCA312D801}" name="sqlserver_start_time_ms_ticks"/>
-    <tableColumn id="19" xr3:uid="{06292E30-63F3-4020-B8C5-BAA3E876F63C}" name="sqlserver_start_time" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{06292E30-63F3-4020-B8C5-BAA3E876F63C}" name="sqlserver_start_time" dataDxfId="17"/>
     <tableColumn id="20" xr3:uid="{E04BAAE3-3FC6-4B59-9C98-426E92F97D81}" name="affinity_type"/>
     <tableColumn id="21" xr3:uid="{F629596F-A9F2-4FB4-83C0-37312548DF18}" name="affinity_type_desc"/>
     <tableColumn id="22" xr3:uid="{8513385E-8766-4E2B-B489-07868FCA0057}" name="process_kernel_time_ms"/>
@@ -1345,6 +1392,37 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}" name="Table11" displayName="Table11" ref="A1:V2" totalsRowShown="0">
+  <autoFilter ref="A1:V2" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}"/>
+  <tableColumns count="22">
+    <tableColumn id="1" xr3:uid="{61888DB5-7723-4C9A-8D5B-C81CCB6ED9E6}" name="database_id"/>
+    <tableColumn id="2" xr3:uid="{A86720A0-06D0-40AD-9F6B-1B855952AC6C}" name="schema_id"/>
+    <tableColumn id="3" xr3:uid="{8F0A9D85-CC5A-4861-A2F3-DDC6CC8CD54C}" name="schema_name"/>
+    <tableColumn id="4" xr3:uid="{C55B07E9-5CFE-441D-9F0B-DF33A9657EB8}" name="object_id"/>
+    <tableColumn id="5" xr3:uid="{044A8FCF-FE45-419A-B079-BFD898725C14}" name="object_name"/>
+    <tableColumn id="6" xr3:uid="{F99F0322-40C6-42BA-9800-F44F58F62D6E}" name="stats_id"/>
+    <tableColumn id="7" xr3:uid="{F1AA4362-02FE-4221-8860-A537DB69E204}" name="stats_name"/>
+    <tableColumn id="8" xr3:uid="{514B7C8E-5B62-4A9D-BF85-9A15452B26D7}" name="auto_created"/>
+    <tableColumn id="9" xr3:uid="{B1676F5F-0FE6-44CB-A8A3-9CAA7649C600}" name="user_created"/>
+    <tableColumn id="10" xr3:uid="{0BD065B3-2D00-4634-872D-46A357183566}" name="no_recompute"/>
+    <tableColumn id="11" xr3:uid="{28D22481-92DB-4B5E-BD30-F719FBC13512}" name="has_filter"/>
+    <tableColumn id="12" xr3:uid="{78D5D7D1-96F0-4CDD-B2A1-E527CCB483AF}" name="filter_definition"/>
+    <tableColumn id="13" xr3:uid="{1ABA3DBF-5D2A-4BBB-98FF-33849B90EB35}" name="is_temporary"/>
+    <tableColumn id="14" xr3:uid="{96E6B6B8-1B2C-4A9D-B210-1AFE5A179C0A}" name="is_incremental"/>
+    <tableColumn id="17" xr3:uid="{38EF12FA-51C5-4EE8-88DD-2B03C7A2C1E6}" name="stats_columns"/>
+    <tableColumn id="18" xr3:uid="{55E4D7C1-B7C8-44B5-AEB9-B5295B0A1B42}" name="last_updated" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{E1068D45-CB37-405C-B69F-3FF11CD0BADF}" name="rows"/>
+    <tableColumn id="20" xr3:uid="{7E666E1D-950B-4E36-BBF2-9EF8063C1503}" name="rows_sampled"/>
+    <tableColumn id="21" xr3:uid="{59FBFE22-CD62-4975-A9B1-C9A117EB6357}" name="steps"/>
+    <tableColumn id="22" xr3:uid="{22D74C0F-E277-43AB-9D30-0D7CC0A032E4}" name="unfiltered_rows"/>
+    <tableColumn id="23" xr3:uid="{DA43F736-BB2D-41A5-8E8E-FF7CDA7CDF03}" name="modification_counter"/>
+    <tableColumn id="24" xr3:uid="{A8C3B7C6-79E3-43DB-9268-186D346ADF85}" name="persisted_sample_percent"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4CAADD08-DBD5-4AD2-AA6D-225DF1B2ECAD}" name="Table12" displayName="Table12" ref="A1:M2" totalsRowShown="0">
   <autoFilter ref="A1:M2" xr:uid="{4CAADD08-DBD5-4AD2-AA6D-225DF1B2ECAD}"/>
   <tableColumns count="13">
@@ -1373,7 +1451,7 @@
     <tableColumn id="1" xr3:uid="{2371C3FF-E1D8-4768-9EB7-0FA51A478EDC}" name="ServerName_s"/>
     <tableColumn id="2" xr3:uid="{7BBA6DC6-36D1-4D30-ADD6-C02E2043FE09}" name="record_id_d"/>
     <tableColumn id="3" xr3:uid="{5FF6B684-4C9B-438D-80AE-420FEDAD3C39}" name="timestamp_d"/>
-    <tableColumn id="4" xr3:uid="{2F0ED155-E681-4A37-8A88-B65DEE436BD4}" name="timestamp_datetime" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{2F0ED155-E681-4A37-8A88-B65DEE436BD4}" name="timestamp_datetime" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{3463BDB4-332F-4798-B2CE-F1047A46AD4C}" name="sql_cpu_d"/>
     <tableColumn id="6" xr3:uid="{13C5E21B-F3D0-48CD-AAEE-22E17DBF17A3}" name="idle_cpu_d"/>
     <tableColumn id="7" xr3:uid="{5EA7BA56-5ED4-4BE5-944F-C0922BC64496}" name="other_cpu_d"/>
@@ -1498,18 +1576,18 @@
     <tableColumn id="5" xr3:uid="{E3C50696-2DF6-484B-9CC5-F6A63497E94B}" name="user_scans"/>
     <tableColumn id="6" xr3:uid="{386BD38C-0AE9-47FC-9B4D-9F4D394ABD8B}" name="user_lookups"/>
     <tableColumn id="7" xr3:uid="{01B932C8-92B8-4277-B3D9-A9AE39577056}" name="user_updates"/>
-    <tableColumn id="8" xr3:uid="{C3E5BE79-FFEF-4B16-9789-5C0044EADC84}" name="last_user_seek" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{11C49885-2A3C-4462-89E4-664D1A59C4B7}" name="last_user_scan" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{E5E4B8AD-F430-49D1-B65A-421E0A7CFDF7}" name="last_user_lookup" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{DC039DE2-C9B9-40BB-B4D5-05EE8C9040B3}" name="last_user_update" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C3E5BE79-FFEF-4B16-9789-5C0044EADC84}" name="last_user_seek" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{11C49885-2A3C-4462-89E4-664D1A59C4B7}" name="last_user_scan" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{E5E4B8AD-F430-49D1-B65A-421E0A7CFDF7}" name="last_user_lookup" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{DC039DE2-C9B9-40BB-B4D5-05EE8C9040B3}" name="last_user_update" dataDxfId="13"/>
     <tableColumn id="12" xr3:uid="{A073FE55-50AC-4479-8C3B-7B25AA30CCAC}" name="system_seeks"/>
     <tableColumn id="13" xr3:uid="{0F6309D4-0D6E-4AD6-AEAE-2A274B502951}" name="system_scans"/>
     <tableColumn id="14" xr3:uid="{DCC3CE1E-11F9-4A50-88F7-FCD8E280010E}" name="system_lookups"/>
     <tableColumn id="15" xr3:uid="{BD0A8475-696B-44D2-81AA-79B5C350A586}" name="system_updates"/>
-    <tableColumn id="16" xr3:uid="{DA729497-0017-44D4-A880-36A2A1972E39}" name="last_system_seek" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{172DA864-2310-4B69-BF7D-E8D9F325F765}" name="last_system_scan" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{019F50A5-DDEA-423E-AAF2-3650EA866E9B}" name="last_system_lookup" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{1D34997E-47AB-4B29-9B50-242BC31D929F}" name="last_system_update" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{DA729497-0017-44D4-A880-36A2A1972E39}" name="last_system_seek" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{172DA864-2310-4B69-BF7D-E8D9F325F765}" name="last_system_scan" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{019F50A5-DDEA-423E-AAF2-3650EA866E9B}" name="last_system_lookup" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{1D34997E-47AB-4B29-9B50-242BC31D929F}" name="last_system_update" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1570,31 +1648,32 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}" name="Table11" displayName="Table11" ref="A1:V2" totalsRowShown="0">
-  <autoFilter ref="A1:V2" xr:uid="{F7580916-697D-4A18-B035-F4624F75B388}"/>
-  <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{61888DB5-7723-4C9A-8D5B-C81CCB6ED9E6}" name="database_id"/>
-    <tableColumn id="2" xr3:uid="{A86720A0-06D0-40AD-9F6B-1B855952AC6C}" name="schema_id"/>
-    <tableColumn id="3" xr3:uid="{8F0A9D85-CC5A-4861-A2F3-DDC6CC8CD54C}" name="schema_name"/>
-    <tableColumn id="4" xr3:uid="{C55B07E9-5CFE-441D-9F0B-DF33A9657EB8}" name="object_id"/>
-    <tableColumn id="5" xr3:uid="{044A8FCF-FE45-419A-B079-BFD898725C14}" name="object_name"/>
-    <tableColumn id="6" xr3:uid="{F99F0322-40C6-42BA-9800-F44F58F62D6E}" name="stats_id"/>
-    <tableColumn id="7" xr3:uid="{F1AA4362-02FE-4221-8860-A537DB69E204}" name="stats_name"/>
-    <tableColumn id="8" xr3:uid="{514B7C8E-5B62-4A9D-BF85-9A15452B26D7}" name="auto_created"/>
-    <tableColumn id="9" xr3:uid="{B1676F5F-0FE6-44CB-A8A3-9CAA7649C600}" name="user_created"/>
-    <tableColumn id="10" xr3:uid="{0BD065B3-2D00-4634-872D-46A357183566}" name="no_recompute"/>
-    <tableColumn id="11" xr3:uid="{28D22481-92DB-4B5E-BD30-F719FBC13512}" name="has_filter"/>
-    <tableColumn id="12" xr3:uid="{78D5D7D1-96F0-4CDD-B2A1-E527CCB483AF}" name="filter_definition"/>
-    <tableColumn id="13" xr3:uid="{1ABA3DBF-5D2A-4BBB-98FF-33849B90EB35}" name="is_temporary"/>
-    <tableColumn id="14" xr3:uid="{96E6B6B8-1B2C-4A9D-B210-1AFE5A179C0A}" name="is_incremental"/>
-    <tableColumn id="17" xr3:uid="{38EF12FA-51C5-4EE8-88DD-2B03C7A2C1E6}" name="stats_columns"/>
-    <tableColumn id="18" xr3:uid="{55E4D7C1-B7C8-44B5-AEB9-B5295B0A1B42}" name="last_updated" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{E1068D45-CB37-405C-B69F-3FF11CD0BADF}" name="rows"/>
-    <tableColumn id="20" xr3:uid="{7E666E1D-950B-4E36-BBF2-9EF8063C1503}" name="rows_sampled"/>
-    <tableColumn id="21" xr3:uid="{59FBFE22-CD62-4975-A9B1-C9A117EB6357}" name="steps"/>
-    <tableColumn id="22" xr3:uid="{22D74C0F-E277-43AB-9D30-0D7CC0A032E4}" name="unfiltered_rows"/>
-    <tableColumn id="23" xr3:uid="{DA43F736-BB2D-41A5-8E8E-FF7CDA7CDF03}" name="modification_counter"/>
-    <tableColumn id="24" xr3:uid="{A8C3B7C6-79E3-43DB-9268-186D346ADF85}" name="persisted_sample_percent"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{338AD530-E0AE-4BF8-91E4-92886203524B}" name="Table2" displayName="Table2" ref="A1:W2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:W2" xr:uid="{338AD530-E0AE-4BF8-91E4-92886203524B}"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{B4B9BFB0-D7B9-44A1-93D7-0F9F60C6AED5}" name="database_id"/>
+    <tableColumn id="2" xr3:uid="{510D877A-A17B-402A-A395-DE12F26B44DA}" name="object_id"/>
+    <tableColumn id="3" xr3:uid="{77EA3CEA-41C1-4879-A431-057B34DB3D62}" name="schema_name"/>
+    <tableColumn id="4" xr3:uid="{79222D62-B59D-4D15-BD4A-5D03AF2C6AE0}" name="object_name"/>
+    <tableColumn id="5" xr3:uid="{3E9B6ADD-F931-4AC7-808F-1B1300B04BE1}" name="index_id"/>
+    <tableColumn id="6" xr3:uid="{190C71B3-F63A-414C-97D0-BB1BAAA77533}" name="index_name"/>
+    <tableColumn id="7" xr3:uid="{044C1191-7BEA-43A6-952C-7AF14B127E54}" name="key_ordinal"/>
+    <tableColumn id="8" xr3:uid="{56581A98-21E9-4BEF-8FB7-9A4AF480944D}" name="column_name" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{CA5AFCED-2427-4579-A9F1-CB0598187D16}" name="sqlserver_start_time" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4E4D1F12-48CF-4312-84A1-9AE0B28F041F}" name="user_seeks"/>
+    <tableColumn id="11" xr3:uid="{FFEAD205-2EED-4BE2-9E2C-061C27307D20}" name="user_scans"/>
+    <tableColumn id="12" xr3:uid="{BFAD7294-E0FB-440F-B56A-85E4D4A76AFC}" name="user_lookups"/>
+    <tableColumn id="13" xr3:uid="{D3381E36-542A-48F9-B45E-743C2A94FA87}" name="user_updates" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{1396F2EB-E4F0-4308-A131-B03356D23533}" name="last_user_seek" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{C9D6A49B-A722-4B7E-8520-1176428B52B0}" name="last_user_scan" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{5F30294C-C6A6-4062-B487-A6C4709293D2}" name="last_user_lookup" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{2DE012F2-9E50-4D07-8E71-4C2C1B2478F8}" name="last_system_update" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{A97D6EED-7F32-43D3-9782-A9AF9C104EE6}" name="avg_distribution"/>
+    <tableColumn id="19" xr3:uid="{BD4BA2D3-25AE-487D-8142-2C38A86443BD}" name="max_distribution"/>
+    <tableColumn id="20" xr3:uid="{F9564677-8714-467A-B0AD-A09A07BF0AE8}" name="avg_distribution_order"/>
+    <tableColumn id="21" xr3:uid="{AD9DAE4F-CBC2-45E8-82DB-1829475B1A03}" name="max_distribution_order"/>
+    <tableColumn id="22" xr3:uid="{459F32F0-8850-4CD2-8FD0-2FF62CF3F46C}" name="order_issue_avg_dist"/>
+    <tableColumn id="23" xr3:uid="{E48A3031-078F-4459-838B-2EAC5757DC95}" name="order_issue_max_dist"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1923,45 +2002,45 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.9296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.1328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.06640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.9296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -2074,104 +2153,116 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5216EEC-EE56-469C-B0AC-60F6560CE05C}">
-  <dimension ref="A1:V1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63ACCF7-ABAC-4D21-AFB1-71ACCED7C200}">
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.53125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.06640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="22" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="H1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" t="s">
-        <v>157</v>
+        <v>182</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="J1" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="L1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M1" t="s">
-        <v>160</v>
-      </c>
-      <c r="N1" t="s">
-        <v>161</v>
-      </c>
-      <c r="O1" t="s">
-        <v>162</v>
+        <v>99</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>38</v>
+        <v>103</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="R1" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="S1" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="T1" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="U1" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="V1" t="s">
-        <v>168</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="W1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2182,6 +2273,114 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5216EEC-EE56-469C-B0AC-60F6560CE05C}">
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
+        <v>161</v>
+      </c>
+      <c r="O1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>164</v>
+      </c>
+      <c r="S1" t="s">
+        <v>165</v>
+      </c>
+      <c r="T1" t="s">
+        <v>166</v>
+      </c>
+      <c r="U1" t="s">
+        <v>167</v>
+      </c>
+      <c r="V1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB8D599-8A21-4C49-8BBE-5F2B5EFE4765}">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -2189,22 +2388,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2255,24 +2454,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE05985A-666D-4AC8-A72E-F67D7A7873A1}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -2282,7 +2481,7 @@
       <c r="C1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>86</v>
       </c>
       <c r="E1" t="s">
@@ -2294,9 +2493,6 @@
       <c r="G1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2314,16 +2510,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -2356,39 +2552,39 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="138.46484375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="138.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.06640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2490,14 +2686,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2505,7 +2701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -2516,12 +2712,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -2536,35 +2732,35 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="75.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.46484375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.46484375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2645,26 +2841,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.53125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2727,29 +2923,29 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13.1328125" customWidth="1"/>
-    <col min="8" max="8" width="14.06640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.19921875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.796875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.9296875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.46484375" customWidth="1"/>
-    <col min="13" max="13" width="13.59765625" customWidth="1"/>
-    <col min="14" max="14" width="15.19921875" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.265625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="16.3984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="14" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" style="4" customWidth="1"/>
     <col min="18" max="18" width="18" style="4" customWidth="1"/>
-    <col min="19" max="19" width="18.1328125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2824,56 +3020,56 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.1328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="29.59765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.53125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.53125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26.06640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.265625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.46484375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.73046875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="30.53125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="30.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>